<commit_message>
feat: add pdf auto-translation for translations
</commit_message>
<xml_diff>
--- a/web/public/templates/translations_template.xlsx
+++ b/web/public/templates/translations_template.xlsx
@@ -1,52 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="translations" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="translations" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,13 +42,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,71 +440,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>매뉴얼ID</v>
-      </c>
-      <c r="B1" t="str">
-        <v>한글제목</v>
-      </c>
-      <c r="C1" t="str">
-        <v>한글요약</v>
-      </c>
-      <c r="D1" t="str">
-        <v>한글본문</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>???ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>????</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>??PDF</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>350d-engine-frontmatter-and-toc-2023-02-15</v>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>350d-engine-frontmatter-and-toc-2023-02-15</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>350d-engine-lubrication-system-2023-02-15</v>
-      </c>
-      <c r="B3" t="str">
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <v/>
-      </c>
-      <c r="D3" t="str">
-        <v/>
-      </c>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>350d-engine-lubrication-system-2023-02-15</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="str">
-        <v>350d-engine-cylinder-head-cover-and-head-2023-02-15</v>
-      </c>
-      <c r="B4" t="str">
-        <v/>
-      </c>
-      <c r="C4" t="str">
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <v/>
-      </c>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>350d-engine-cylinder-head-cover-and-head-2023-02-15</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>